<commit_message>
all feature works very well!!!
</commit_message>
<xml_diff>
--- a/apFilter/apFilterPdf/ACH.xlsx
+++ b/apFilter/apFilterPdf/ACH.xlsx
@@ -1,48 +1,79 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Month</t>
   </si>
   <si>
-    <t>vendor name</t>
-  </si>
-  <si>
-    <t>transaction date</t>
-  </si>
-  <si>
-    <t>local payday</t>
-  </si>
-  <si>
-    <t>amount</t>
-  </si>
-  <si>
-    <t>paytype</t>
-  </si>
-  <si>
-    <t>ap number</t>
-  </si>
-  <si>
-    <t>remin date</t>
+    <t>Remin Date</t>
+  </si>
+  <si>
+    <t>AP NO.</t>
+  </si>
+  <si>
+    <t>Vender Name</t>
+  </si>
+  <si>
+    <t>Transaction date</t>
+  </si>
+  <si>
+    <t>Local Payday</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>20201015</t>
+  </si>
+  <si>
+    <t>20201005-ZSAC-0005</t>
+  </si>
+  <si>
+    <t>AERO PERFORMANCE</t>
+  </si>
+  <si>
+    <t>20201007</t>
+  </si>
+  <si>
+    <t>20201005-ZSAC-0006</t>
+  </si>
+  <si>
+    <t>DUNCAN AVIATION</t>
+  </si>
+  <si>
+    <t>20201005-ZSAC-0007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WILLIS TOWERS WATSON INSURANCE SERVICES WEST, </t>
+  </si>
+  <si>
+    <t>20201005-ZSAC-0008</t>
+  </si>
+  <si>
+    <t>AIRCRAFT SPRUCE &amp; SPECIALTY CO.</t>
+  </si>
+  <si>
+    <t>20201013</t>
+  </si>
+  <si>
+    <t>20201005-ZSAC-0009</t>
+  </si>
+  <si>
+    <t>ADAM JEHN DUNG TSUEI</t>
   </si>
 </sst>
 </file>
@@ -51,11 +82,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -78,8 +109,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,45 +394,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="4" max="4" width="49.85546875" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>4</v>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2">
+        <v>55827.44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>26.83</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5">
+        <v>1069.95</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6">
+        <v>3921.06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add the modular punchInOut which can process the personal system's punch in and out report
</commit_message>
<xml_diff>
--- a/apFilter/apFilterPdf/ACH.xlsx
+++ b/apFilter/apFilterPdf/ACH.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>Month</t>
   </si>
@@ -74,6 +74,27 @@
   </si>
   <si>
     <t>ADAM JEHN DUNG TSUEI</t>
+  </si>
+  <si>
+    <t>20201008-ZSAC-0001</t>
+  </si>
+  <si>
+    <t>20201009</t>
+  </si>
+  <si>
+    <t>20201008-ZSAC-0002</t>
+  </si>
+  <si>
+    <t>CELEBRATION TOURS &amp; TRAVEL</t>
+  </si>
+  <si>
+    <t>20201008-ZSAC-0003</t>
+  </si>
+  <si>
+    <t>MULTI SERVICE AVIATION</t>
+  </si>
+  <si>
+    <t>20201014</t>
   </si>
 </sst>
 </file>
@@ -82,11 +103,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -394,13 +415,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
@@ -432,7 +453,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -449,7 +470,7 @@
         <v>55827.44</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -466,7 +487,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -483,7 +504,7 @@
         <v>26.83</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -500,7 +521,7 @@
         <v>1069.95</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -515,6 +536,57 @@
       </c>
       <c r="G6">
         <v>3921.06</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7">
+        <v>216.83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8">
+        <v>14650</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9">
+        <v>6185.47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add folder parseCOA4Bugget, the project under this folder is for quick query account code/ item code basing on the given item code /account code.
</commit_message>
<xml_diff>
--- a/apFilter/apFilterPdf/ACH.xlsx
+++ b/apFilter/apFilterPdf/ACH.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>Month</t>
   </si>
@@ -418,7 +418,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N26" sqref="N26"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,8 +463,8 @@
       <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
+      <c r="F2">
+        <v>20201005</v>
       </c>
       <c r="G2">
         <v>55827.44</v>

</xml_diff>

<commit_message>
adFilterPdf add special case for parsing 4601 which has no localPayDay; add special case for vendor is employee which code is only 6 digit
</commit_message>
<xml_diff>
--- a/apFilter/apFilterPdf/ACH.xlsx
+++ b/apFilter/apFilterPdf/ACH.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="54">
   <si>
     <t>Month</t>
   </si>
@@ -46,15 +46,15 @@
     <t>AERO PERFORMANCE</t>
   </si>
   <si>
+    <t>20201005-ZSAC-0006</t>
+  </si>
+  <si>
+    <t>DUNCAN AVIATION</t>
+  </si>
+  <si>
     <t>20201007</t>
   </si>
   <si>
-    <t>20201005-ZSAC-0006</t>
-  </si>
-  <si>
-    <t>DUNCAN AVIATION</t>
-  </si>
-  <si>
     <t>20201005-ZSAC-0007</t>
   </si>
   <si>
@@ -95,6 +95,87 @@
   </si>
   <si>
     <t>20201014</t>
+  </si>
+  <si>
+    <t>20201030</t>
+  </si>
+  <si>
+    <t>20201012-ZSAC-0004</t>
+  </si>
+  <si>
+    <t>ALLIED RECEIVABLES FUNDING INC.</t>
+  </si>
+  <si>
+    <t>20201016</t>
+  </si>
+  <si>
+    <t>20201012-ZSAC-0005</t>
+  </si>
+  <si>
+    <t>ADP, LLC</t>
+  </si>
+  <si>
+    <t>20201012-ZSAC-0006</t>
+  </si>
+  <si>
+    <t>ALLSTREAM</t>
+  </si>
+  <si>
+    <t>20201020</t>
+  </si>
+  <si>
+    <t>20201012-ZSAC-0007</t>
+  </si>
+  <si>
+    <t>S&amp;D CARWASH MANAGEMENT, LLC</t>
+  </si>
+  <si>
+    <t>20201028</t>
+  </si>
+  <si>
+    <t>20201012-ZSAC-0008</t>
+  </si>
+  <si>
+    <t>EVA AIRWAYS CORPORATION</t>
+  </si>
+  <si>
+    <t>20201012-ZSAC-0009</t>
+  </si>
+  <si>
+    <t>FLIGHT TRAINING ACADEMY</t>
+  </si>
+  <si>
+    <t>20201012-ZSAC-0010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIDELITY INVESTMENTS INSTITUTIONAL SERVICES </t>
+  </si>
+  <si>
+    <t>20201012-ZSAC-0011</t>
+  </si>
+  <si>
+    <t>ANTHEM BLUE CROSS</t>
+  </si>
+  <si>
+    <t>20201012-ZSAC-0012</t>
+  </si>
+  <si>
+    <t>20201012-ZSAC-0013</t>
+  </si>
+  <si>
+    <t>李豪傑</t>
+  </si>
+  <si>
+    <t>20201012-ZSAC-0014</t>
+  </si>
+  <si>
+    <t>RAMOS OIL COMPANY</t>
+  </si>
+  <si>
+    <t>20201012</t>
+  </si>
+  <si>
+    <t>20201012-ZSAC-4601</t>
   </si>
 </sst>
 </file>
@@ -103,11 +184,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -415,13 +496,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
@@ -453,7 +534,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -470,24 +551,24 @@
         <v>55827.44</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
       </c>
       <c r="G3">
         <v>1200</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -498,13 +579,13 @@
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G4">
         <v>26.83</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -521,7 +602,7 @@
         <v>1069.95</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -538,7 +619,7 @@
         <v>3921.06</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -555,7 +636,7 @@
         <v>216.83</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -572,7 +653,7 @@
         <v>14650</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -587,6 +668,210 @@
       </c>
       <c r="G9">
         <v>6185.47</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10">
+        <v>116.4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11">
+        <v>206.45</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12">
+        <v>1299.7</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13">
+        <v>88.99</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>40</v>
+      </c>
+      <c r="F14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14">
+        <v>3040</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15">
+        <v>84493.56</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>44</v>
+      </c>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16">
+        <v>5921.73</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17">
+        <v>502.53</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
+      </c>
+      <c r="F18" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18">
+        <v>8952.45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" t="s">
+        <v>26</v>
+      </c>
+      <c r="G19">
+        <v>580.39</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20" t="s">
+        <v>52</v>
+      </c>
+      <c r="G20">
+        <v>1782.3</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F21">
+        <v>20201014</v>
+      </c>
+      <c r="G21">
+        <v>4083.35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
transaction list need more time
</commit_message>
<xml_diff>
--- a/apFilter/apFilterPdf/ACH.xlsx
+++ b/apFilter/apFilterPdf/ACH.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -184,11 +184,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -498,11 +498,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
@@ -534,7 +534,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -551,7 +551,7 @@
         <v>55827.44</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -568,7 +568,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -585,7 +585,7 @@
         <v>26.83</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -602,7 +602,7 @@
         <v>1069.95</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -619,7 +619,7 @@
         <v>3921.06</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -636,7 +636,7 @@
         <v>216.83</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -653,7 +653,7 @@
         <v>14650</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -670,7 +670,7 @@
         <v>6185.47</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>27</v>
       </c>
@@ -687,7 +687,7 @@
         <v>116.4</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -704,7 +704,7 @@
         <v>206.45</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>27</v>
       </c>
@@ -721,7 +721,7 @@
         <v>1299.7</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>27</v>
       </c>
@@ -738,7 +738,7 @@
         <v>88.99</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>27</v>
       </c>
@@ -755,7 +755,7 @@
         <v>3040</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -772,7 +772,7 @@
         <v>84493.56</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>7</v>
       </c>
@@ -820,7 +820,7 @@
         <v>17</v>
       </c>
       <c r="G18">
-        <v>8952.45</v>
+        <v>8952.4500000000007</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Now, the application can address the amount combination. I still need some time to digest the core function which I copied from stack overflow:)
</commit_message>
<xml_diff>
--- a/apFilter/apFilterPdf/ACH.xlsx
+++ b/apFilter/apFilterPdf/ACH.xlsx
@@ -9,12 +9,16 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$21</definedName>
+    <definedName name="_xlnm._FilterDatabase">Sheet1!$A$1:$G$21</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
   <si>
     <t>Month</t>
   </si>
@@ -211,8 +215,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -499,7 +504,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:F4"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,6 +514,7 @@
     <col min="4" max="4" width="49.85546875" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -518,7 +524,7 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
@@ -530,7 +536,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -547,7 +553,7 @@
       <c r="F2">
         <v>20201005</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>55827.44</v>
       </c>
     </row>
@@ -561,10 +567,13 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
       <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>1200</v>
       </c>
     </row>
@@ -578,10 +587,13 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
       <c r="F4" t="s">
         <v>12</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="1">
         <v>26.83</v>
       </c>
     </row>
@@ -595,10 +607,13 @@
       <c r="D5" t="s">
         <v>16</v>
       </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
       <c r="F5" t="s">
         <v>17</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>1069.95</v>
       </c>
     </row>
@@ -612,10 +627,13 @@
       <c r="D6" t="s">
         <v>19</v>
       </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
       <c r="F6" t="s">
         <v>17</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>3921.06</v>
       </c>
     </row>
@@ -632,7 +650,7 @@
       <c r="F7" t="s">
         <v>21</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>216.83</v>
       </c>
     </row>
@@ -646,10 +664,13 @@
       <c r="D8" t="s">
         <v>23</v>
       </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
       <c r="F8" t="s">
         <v>17</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <v>14650</v>
       </c>
     </row>
@@ -666,7 +687,7 @@
       <c r="F9" t="s">
         <v>26</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>6185.47</v>
       </c>
     </row>
@@ -683,7 +704,7 @@
       <c r="F10" t="s">
         <v>30</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="1">
         <v>116.4</v>
       </c>
     </row>
@@ -700,7 +721,7 @@
       <c r="F11" t="s">
         <v>21</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="1">
         <v>206.45</v>
       </c>
     </row>
@@ -717,7 +738,7 @@
       <c r="F12" t="s">
         <v>35</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="1">
         <v>1299.7</v>
       </c>
     </row>
@@ -734,7 +755,7 @@
       <c r="F13" t="s">
         <v>38</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="1">
         <v>88.99</v>
       </c>
     </row>
@@ -751,7 +772,7 @@
       <c r="F14" t="s">
         <v>38</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="1">
         <v>3040</v>
       </c>
     </row>
@@ -768,7 +789,7 @@
       <c r="F15" t="s">
         <v>26</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="1">
         <v>84493.56</v>
       </c>
     </row>
@@ -782,10 +803,13 @@
       <c r="D16" t="s">
         <v>44</v>
       </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
       <c r="F16" t="s">
         <v>17</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="1">
         <v>5921.73</v>
       </c>
     </row>
@@ -799,10 +823,13 @@
       <c r="D17" t="s">
         <v>46</v>
       </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
       <c r="F17" t="s">
         <v>17</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="1">
         <v>502.53</v>
       </c>
     </row>
@@ -816,10 +843,13 @@
       <c r="D18" t="s">
         <v>42</v>
       </c>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
       <c r="F18" t="s">
         <v>17</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
         <v>8952.4500000000007</v>
       </c>
     </row>
@@ -836,7 +866,7 @@
       <c r="F19" t="s">
         <v>26</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="1">
         <v>580.39</v>
       </c>
     </row>
@@ -850,10 +880,13 @@
       <c r="D20" t="s">
         <v>51</v>
       </c>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
       <c r="F20" t="s">
         <v>52</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="1">
         <v>1782.3</v>
       </c>
     </row>
@@ -870,11 +903,13 @@
       <c r="F21">
         <v>20201014</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="1">
         <v>4083.35</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G21"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add comments to help future reviewing
</commit_message>
<xml_diff>
--- a/apFilter/apFilterPdf/ACH.xlsx
+++ b/apFilter/apFilterPdf/ACH.xlsx
@@ -10,15 +10,15 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$26</definedName>
     <definedName name="_xlnm._FilterDatabase">Sheet1!$A$1:$G$21</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="61">
   <si>
     <t>Month</t>
   </si>
@@ -180,6 +180,27 @@
   </si>
   <si>
     <t>20201012-ZSAC-4601</t>
+  </si>
+  <si>
+    <t>20201014-ZSAC-0004</t>
+  </si>
+  <si>
+    <t>CINTAS CORPORATION</t>
+  </si>
+  <si>
+    <t>20201014-ZSAC-0005</t>
+  </si>
+  <si>
+    <t>CALIFORNIA DEPARTMENT OF TAX AND FEE ADMINISTRATION</t>
+  </si>
+  <si>
+    <t>20201023</t>
+  </si>
+  <si>
+    <t>20201014-ZSAC-0006</t>
+  </si>
+  <si>
+    <t>20201021</t>
   </si>
 </sst>
 </file>
@@ -501,17 +522,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="49.85546875" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" customWidth="1"/>
     <col min="7" max="7" width="10.140625" style="1" customWidth="1"/>
@@ -684,6 +705,9 @@
       <c r="D9" t="s">
         <v>25</v>
       </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
       <c r="F9" t="s">
         <v>26</v>
       </c>
@@ -786,6 +810,9 @@
       <c r="D15" t="s">
         <v>42</v>
       </c>
+      <c r="E15" t="s">
+        <v>26</v>
+      </c>
       <c r="F15" t="s">
         <v>26</v>
       </c>
@@ -813,7 +840,7 @@
         <v>5921.73</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>7</v>
       </c>
@@ -833,7 +860,7 @@
         <v>502.53</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>7</v>
       </c>
@@ -853,7 +880,7 @@
         <v>8952.4500000000007</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>7</v>
       </c>
@@ -863,6 +890,9 @@
       <c r="D19" t="s">
         <v>49</v>
       </c>
+      <c r="E19" t="s">
+        <v>26</v>
+      </c>
       <c r="F19" t="s">
         <v>26</v>
       </c>
@@ -870,7 +900,7 @@
         <v>580.39</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>7</v>
       </c>
@@ -890,7 +920,7 @@
         <v>1782.3</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>7</v>
       </c>
@@ -900,6 +930,9 @@
       <c r="D21" t="s">
         <v>42</v>
       </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
       <c r="F21">
         <v>20201014</v>
       </c>
@@ -907,8 +940,65 @@
         <v>4083.35</v>
       </c>
     </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1221.3699999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" s="1">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" t="s">
+        <v>25</v>
+      </c>
+      <c r="F24" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24" s="1">
+        <v>7017.59</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="J26" s="1"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G21"/>
+  <autoFilter ref="A1:G26"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="0"/>
 </worksheet>

</xml_diff>

<commit_message>
General Voucher Can be keyed in automatically Now, I want to have a frontend
</commit_message>
<xml_diff>
--- a/apFilter/apFilterPdf/ACH.xlsx
+++ b/apFilter/apFilterPdf/ACH.xlsx
@@ -524,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -725,6 +725,9 @@
       <c r="D10" t="s">
         <v>29</v>
       </c>
+      <c r="E10">
+        <v>20201016</v>
+      </c>
       <c r="F10" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
fix a bug when the amount is negative, the parsing will show as (34.32) and there is no space in el[0],split will fail
</commit_message>
<xml_diff>
--- a/apFilter/apFilterPdf/ACH.xlsx
+++ b/apFilter/apFilterPdf/ACH.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Sheet1" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$26</definedName>
     <definedName name="_xlnm._FilterDatabase">Sheet1!$A$1:$G$21</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="71">
   <si>
     <t>Month</t>
   </si>
@@ -201,6 +200,36 @@
   </si>
   <si>
     <t>20201021</t>
+  </si>
+  <si>
+    <t>20201020-ZSAC-0009</t>
+  </si>
+  <si>
+    <t>20201020-ZSAC-0010</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHASE BANK SACRAMENTO-FLORIN WEST </t>
+  </si>
+  <si>
+    <t>20201020-ZSAC-0011</t>
+  </si>
+  <si>
+    <t>WILLIS TOWERS WATSON NORTHEAST, INC</t>
+  </si>
+  <si>
+    <t>20201020-ZSAC-0012</t>
+  </si>
+  <si>
+    <t>WELLS FARGO</t>
+  </si>
+  <si>
+    <t>20201020-ZSAC-0013</t>
+  </si>
+  <si>
+    <t>20201020-ZSAC-0014</t>
+  </si>
+  <si>
+    <t>20201029</t>
   </si>
 </sst>
 </file>
@@ -209,11 +238,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -522,17 +551,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J26"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0" zoomScale="145" zoomScaleNormal="145">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.42578125" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" customWidth="1"/>
     <col min="7" max="7" width="10.140625" style="1" customWidth="1"/>
@@ -561,7 +590,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -578,7 +607,7 @@
         <v>55827.44</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -598,7 +627,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>7</v>
       </c>
@@ -618,7 +647,7 @@
         <v>26.83</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -638,7 +667,7 @@
         <v>1069.95</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -658,7 +687,7 @@
         <v>3921.06</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -675,7 +704,7 @@
         <v>216.83</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>7</v>
       </c>
@@ -695,7 +724,7 @@
         <v>14650</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -715,7 +744,7 @@
         <v>6185.47</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>27</v>
       </c>
@@ -735,7 +764,7 @@
         <v>116.4</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>7</v>
       </c>
@@ -752,7 +781,7 @@
         <v>206.45</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>27</v>
       </c>
@@ -762,6 +791,9 @@
       <c r="D12" t="s">
         <v>34</v>
       </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
       <c r="F12" t="s">
         <v>35</v>
       </c>
@@ -769,7 +801,7 @@
         <v>1299.7</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>27</v>
       </c>
@@ -786,7 +818,7 @@
         <v>88.99</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>27</v>
       </c>
@@ -803,7 +835,7 @@
         <v>3040</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>7</v>
       </c>
@@ -823,7 +855,7 @@
         <v>84493.56</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>7</v>
       </c>
@@ -843,7 +875,7 @@
         <v>5921.73</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>7</v>
       </c>
@@ -863,7 +895,7 @@
         <v>502.53</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>7</v>
       </c>
@@ -880,10 +912,10 @@
         <v>17</v>
       </c>
       <c r="G18" s="1">
-        <v>8952.4500000000007</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+        <v>8952.45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>7</v>
       </c>
@@ -903,7 +935,7 @@
         <v>580.39</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>7</v>
       </c>
@@ -923,7 +955,7 @@
         <v>1782.3</v>
       </c>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>7</v>
       </c>
@@ -943,7 +975,7 @@
         <v>4083.35</v>
       </c>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>27</v>
       </c>
@@ -960,10 +992,10 @@
         <v>26</v>
       </c>
       <c r="G22" s="1">
-        <v>1221.3699999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+        <v>1221.37</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>27</v>
       </c>
@@ -980,7 +1012,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>27</v>
       </c>
@@ -997,12 +1029,110 @@
         <v>7017.59</v>
       </c>
     </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="J26" s="1"/>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" t="s">
+        <v>32</v>
+      </c>
+      <c r="F25" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="1">
+        <v>37.38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" s="1">
+        <v>283.33</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" t="s">
+        <v>64</v>
+      </c>
+      <c r="D27" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" t="s">
+        <v>38</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" t="s">
+        <v>67</v>
+      </c>
+      <c r="F28" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="1">
+        <v>517.52</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" s="1">
+        <v>6509.43</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D30" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G30" s="1">
+        <v>2212.71</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G26"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="0" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adjust the gvInput function. Now, I can free copy paste in excel because I can expand the description columns
</commit_message>
<xml_diff>
--- a/apFilter/apFilterPdf/ACH.xlsx
+++ b/apFilter/apFilterPdf/ACH.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="93">
   <si>
     <t>Month</t>
   </si>
@@ -230,6 +230,72 @@
   </si>
   <si>
     <t>20201029</t>
+  </si>
+  <si>
+    <t>20201026-ZSAC-0001</t>
+  </si>
+  <si>
+    <t>20201026-ZSAC-0002</t>
+  </si>
+  <si>
+    <t>20201026-ZSAC-0003</t>
+  </si>
+  <si>
+    <t>20201026-ZSAC-0004</t>
+  </si>
+  <si>
+    <t>0R011</t>
+  </si>
+  <si>
+    <t>20201113</t>
+  </si>
+  <si>
+    <t>20201026-ZSAC-0006</t>
+  </si>
+  <si>
+    <t>20201104</t>
+  </si>
+  <si>
+    <t>20201026-ZSAC-0007</t>
+  </si>
+  <si>
+    <t>TALON SYSTEMS, LLC</t>
+  </si>
+  <si>
+    <t>20201027-ZSAC-0003</t>
+  </si>
+  <si>
+    <t>20201027-ZSAC-0004</t>
+  </si>
+  <si>
+    <t>20201027-ZSAC-0005</t>
+  </si>
+  <si>
+    <t>20201022-ZSAC-0005</t>
+  </si>
+  <si>
+    <t>BOEING DISTRIBUTION INC</t>
+  </si>
+  <si>
+    <t>20201026</t>
+  </si>
+  <si>
+    <t>20201022-ZSAC-0006</t>
+  </si>
+  <si>
+    <t>DIAMOND AIRCRAFT INDUSTRIES,INC</t>
+  </si>
+  <si>
+    <t>20201022-ZSAC-0007</t>
+  </si>
+  <si>
+    <t>20201022</t>
+  </si>
+  <si>
+    <t>20201022-ZSAC-0008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNITED HEALTH CARE SERVICES INC., UHS PREMIUM </t>
   </si>
 </sst>
 </file>
@@ -551,7 +617,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="145" zoomScaleNormal="145">
       <selection activeCell="D33" sqref="D33"/>
@@ -811,6 +877,9 @@
       <c r="D13" t="s">
         <v>37</v>
       </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
       <c r="F13" t="s">
         <v>38</v>
       </c>
@@ -828,6 +897,9 @@
       <c r="D14" t="s">
         <v>40</v>
       </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
       <c r="F14" t="s">
         <v>38</v>
       </c>
@@ -1005,6 +1077,9 @@
       <c r="D23" t="s">
         <v>57</v>
       </c>
+      <c r="E23" t="s">
+        <v>58</v>
+      </c>
       <c r="F23" t="s">
         <v>58</v>
       </c>
@@ -1022,6 +1097,9 @@
       <c r="D24" t="s">
         <v>25</v>
       </c>
+      <c r="E24" t="s">
+        <v>60</v>
+      </c>
       <c r="F24" t="s">
         <v>60</v>
       </c>
@@ -1090,6 +1168,9 @@
       <c r="D28" t="s">
         <v>67</v>
       </c>
+      <c r="E28" t="s">
+        <v>38</v>
+      </c>
       <c r="F28" t="s">
         <v>38</v>
       </c>
@@ -1107,6 +1188,9 @@
       <c r="D29" t="s">
         <v>25</v>
       </c>
+      <c r="E29" t="s">
+        <v>38</v>
+      </c>
       <c r="F29" t="s">
         <v>38</v>
       </c>
@@ -1129,6 +1213,236 @@
       </c>
       <c r="G30" s="1">
         <v>2212.71</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E31" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" t="s">
+        <v>58</v>
+      </c>
+      <c r="G31" s="1">
+        <v>211.75</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" t="s">
+        <v>72</v>
+      </c>
+      <c r="D32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32" s="1">
+        <v>6031.18</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" t="s">
+        <v>73</v>
+      </c>
+      <c r="D33" t="s">
+        <v>42</v>
+      </c>
+      <c r="F33" t="s">
+        <v>70</v>
+      </c>
+      <c r="G33" s="1">
+        <v>73382.64</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" t="s">
+        <v>75</v>
+      </c>
+      <c r="F34" t="s">
+        <v>70</v>
+      </c>
+      <c r="G34" s="1">
+        <v>17100</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" t="s">
+        <v>78</v>
+      </c>
+      <c r="G35" s="1">
+        <v>7655.98</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" t="s">
+        <v>79</v>
+      </c>
+      <c r="D36" t="s">
+        <v>80</v>
+      </c>
+      <c r="F36" t="s">
+        <v>78</v>
+      </c>
+      <c r="G36" s="1">
+        <v>1527.5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" t="s">
+        <v>40</v>
+      </c>
+      <c r="F37" t="s">
+        <v>70</v>
+      </c>
+      <c r="G37" s="1">
+        <v>23100</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" t="s">
+        <v>40</v>
+      </c>
+      <c r="F38" t="s">
+        <v>78</v>
+      </c>
+      <c r="G38" s="1">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" t="s">
+        <v>65</v>
+      </c>
+      <c r="F39" t="s">
+        <v>27</v>
+      </c>
+      <c r="G39" s="1">
+        <v>4752</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40" t="s">
+        <v>85</v>
+      </c>
+      <c r="F40" t="s">
+        <v>86</v>
+      </c>
+      <c r="G40" s="1">
+        <v>549.61</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" t="s">
+        <v>87</v>
+      </c>
+      <c r="D41" t="s">
+        <v>88</v>
+      </c>
+      <c r="F41" t="s">
+        <v>86</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" t="s">
+        <v>75</v>
+      </c>
+      <c r="F42" t="s">
+        <v>90</v>
+      </c>
+      <c r="G42" s="1">
+        <v>77.44</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" t="s">
+        <v>92</v>
+      </c>
+      <c r="E43" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43" t="s">
+        <v>38</v>
+      </c>
+      <c r="G43" s="1">
+        <v>18946.78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>